<commit_message>
update activity file upload
</commit_message>
<xml_diff>
--- a/public/fileupload/Test_Doctor/Book1.xlsx
+++ b/public/fileupload/Test_Doctor/Book1.xlsx
@@ -1,59 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fileFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOH_Admin\Desktop\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81F8848D-E826-44B0-916B-C0410AC9153B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{BB65D339-D3C7-4DF8-9302-74570ADCD5FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
-  <si>
-    <t>sdsd</t>
-  </si>
-  <si>
-    <t>dsd</t>
-  </si>
-  <si>
-    <t>sdsdsd</t>
-  </si>
-  <si>
-    <t>ggfdgfdfg</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-  <si>
-    <t>dfgdfg</t>
-  </si>
-  <si>
-    <t>dfgdfgdfg</t>
-  </si>
-  <si>
-    <t>dfgd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>xcsdfsdf</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>sdfsdfsdf</t>
+  </si>
+  <si>
+    <t>sdfsdfsd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,7 +120,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -131,7 +132,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -178,6 +179,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -213,6 +231,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -364,95 +399,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8555F9AB-DD02-41DC-AC0A-46D295D0A983}">
+  <dimension ref="A4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>0</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>